<commit_message>
feat: DeepL usage added
</commit_message>
<xml_diff>
--- a/output/frequent_words/xls/all_websites_frequent_words_dict.xlsx
+++ b/output/frequent_words/xls/all_websites_frequent_words_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,328 +456,399 @@
           <t>https://fuckhead.at</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Eat</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://interstellarrecords.at</t>
+          <t>https://fuckhead.at</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Interstellar</t>
+          <t>Immer</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://interstellarrecords.at</t>
+          <t>https://fuckhead.at</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Records</t>
+          <t>Kapital</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://interstellarrecords.at</t>
+          <t>https://fuckhead.at</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Release</t>
+          <t>Piketty</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>https://fuckhead.at</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rich</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>https://interstellarrecords.at</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>New</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>https://interstellarrecords.at</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Interstellar</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://kuprosauwald.org</t>
+          <t>https://interstellarrecords.at</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Obernberg</t>
+          <t>Records</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://kuprosauwald.org</t>
+          <t>https://interstellarrecords.at</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gespeichert</t>
+          <t>Release</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://kuprosauwald.org</t>
+          <t>https://interstellarrecords.at</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Burg</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>https://interstellarrecords.at</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>https://kuprosauwald.org</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Petra</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://kuprosauwald.org</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Oktober</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Obernberg</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://röda.at</t>
+          <t>https://kuprosauwald.org</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Speicherung</t>
+          <t>Gespeichert</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://röda.at</t>
+          <t>https://kuprosauwald.org</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Technische</t>
+          <t>Burg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://röda.at</t>
+          <t>https://kuprosauwald.org</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Zugriff</t>
+          <t>Petra</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>https://kuprosauwald.org</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Oktober</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>https://röda.at</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Zweck</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>https://röda.at</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Uhr</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Speicherung</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://grgr.at</t>
+          <t>https://röda.at</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Gregor</t>
+          <t>Technische</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://grgr.at</t>
+          <t>https://röda.at</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Work</t>
+          <t>Zugriff</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://grgr.at</t>
+          <t>https://röda.at</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Göttfert</t>
+          <t>Zweck</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>https://röda.at</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Uhr</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>https://grgr.at</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Gregor</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://grgr.at</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Work</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://grgr.at</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Göttfert</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://grgr.at</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Posted</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="C29" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>https://grgr.at</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>Installation</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="C30" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>